<commit_message>
09-08-2025 new created programs
</commit_message>
<xml_diff>
--- a/Excelsheet/Anuradha.xlsx
+++ b/Excelsheet/Anuradha.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>username</t>
   </si>
@@ -32,10 +32,7 @@
     <t>pwd</t>
   </si>
   <si>
-    <t>anuradhadabhole5020@gmail.com</t>
-  </si>
-  <si>
-    <t>#@nu_dabhole1707</t>
+    <t>bhfkjhdwkh</t>
   </si>
 </sst>
 </file>
@@ -367,7 +364,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -385,17 +382,17 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
+      <c r="A2" s="1">
+        <v>86577477384</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId1" display="anuradhadabhole5020@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="#@nu_dabhole1707"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>